<commit_message>
Fixed tests after dynamic pollutant/sector implementation
</commit_message>
<xml_diff>
--- a/logic/test/data/_input/05_model_parameters/code_conversions.xlsx
+++ b/logic/test/data/_input/05_model_parameters/code_conversions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Unit_RMA\MAP\_Modellen\E-MAP\05_Runs\_input\05_model_parameters\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RMABuild\emap\logic\test\data\_input\05_model_parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0EBF2F2-0E88-48E5-A271-33D8EB7067DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E34B9D1-3F23-4EEC-997A-353F60565117}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="850" yWindow="-110" windowWidth="37660" windowHeight="21820" activeTab="2" xr2:uid="{12251410-17C7-4612-87CA-5DF1EC65E2D3}"/>
+    <workbookView xWindow="23160" yWindow="1630" windowWidth="13660" windowHeight="16840" xr2:uid="{12251410-17C7-4612-87CA-5DF1EC65E2D3}"/>
   </bookViews>
   <sheets>
     <sheet name="pollutant" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="216">
   <si>
     <t>CO</t>
   </si>
@@ -660,9 +660,6 @@
     <t>1A3bvii(fu)</t>
   </si>
   <si>
-    <t>prioriteit</t>
-  </si>
-  <si>
     <t>Prioriteit = welke code wordt gebruikt indien verschillende codes ingevuld zijn (hoog = meer prioriteit), bv. (fu) wordt gebruikt indien ingevuld</t>
   </si>
   <si>
@@ -673,6 +670,21 @@
   </si>
   <si>
     <t>C_OtherStatComb</t>
+  </si>
+  <si>
+    <t>NFR_priority</t>
+  </si>
+  <si>
+    <t>PCB</t>
+  </si>
+  <si>
+    <t>benzo(b)</t>
+  </si>
+  <si>
+    <t>benzo(k)</t>
+  </si>
+  <si>
+    <t>PCDD/ PCDF</t>
   </si>
 </sst>
 </file>
@@ -743,8 +755,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8B39CD43-4866-4C3B-A178-A99FF32F0A59}" name="tbl_pollutant" displayName="tbl_pollutant" ref="A1:B37" totalsRowShown="0">
-  <autoFilter ref="A1:B37" xr:uid="{0DE66D0D-5368-447A-8271-C03336321777}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8B39CD43-4866-4C3B-A178-A99FF32F0A59}" name="tbl_pollutant" displayName="tbl_pollutant" ref="A1:B40" totalsRowShown="0">
+  <autoFilter ref="A1:B40" xr:uid="{0DE66D0D-5368-447A-8271-C03336321777}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{9514C98B-B8D5-45BC-ADB2-ACBD4CE319C1}" name="pollutant_code"/>
     <tableColumn id="2" xr3:uid="{2AE8A41A-C1EE-4738-B98A-B5A89D38B9B1}" name="pollutant_names"/>
@@ -759,7 +771,7 @@
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{6B25390A-63E3-40F9-84C1-A7A2AC040592}" name="NFR_code"/>
     <tableColumn id="2" xr3:uid="{ECCCA51A-7F4A-4651-8972-626FD9996640}" name="NFR_names"/>
-    <tableColumn id="3" xr3:uid="{41D8043F-6F5E-4F41-968C-90143809976A}" name="prioriteit"/>
+    <tableColumn id="3" xr3:uid="{41D8043F-6F5E-4F41-968C-90143809976A}" name="NFR_priority"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -1073,16 +1085,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{157BD3C6-51C2-4B17-80FA-10EB7A062B80}">
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.54296875" customWidth="1"/>
-    <col min="2" max="2" width="18.1796875" customWidth="1"/>
+    <col min="1" max="1" width="23.7265625" customWidth="1"/>
+    <col min="2" max="2" width="27.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -1146,7 +1158,7 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
@@ -1250,135 +1262,159 @@
         <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>26</v>
+        <v>215</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B22" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B23" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B24" t="s">
-        <v>32</v>
+        <v>213</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B25" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B26" t="s">
-        <v>36</v>
+        <v>214</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B27" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B28" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>5</v>
+        <v>38</v>
       </c>
       <c r="B30" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>2</v>
+        <v>39</v>
       </c>
       <c r="B31" t="s">
-        <v>4</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="B32" t="s">
-        <v>5</v>
+        <v>212</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B33" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B34" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B35" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="B36" t="s">
-        <v>37</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B37" t="s">
-        <v>4</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>11</v>
+      </c>
+      <c r="B38" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>11</v>
+      </c>
+      <c r="B39" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>35</v>
+      </c>
+      <c r="B40" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1395,13 +1431,14 @@
   <dimension ref="A1:E135"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="19.1796875" customWidth="1"/>
     <col min="2" max="2" width="13.54296875" customWidth="1"/>
+    <col min="3" max="3" width="14.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -1412,7 +1449,7 @@
         <v>170</v>
       </c>
       <c r="C1" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -1426,7 +1463,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -2904,7 +2941,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BA1389C-35B1-417E-B6AE-DDCDA0344782}">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -2951,7 +2988,7 @@
         <v>188</v>
       </c>
       <c r="B5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -2967,7 +3004,7 @@
         <v>189</v>
       </c>
       <c r="B7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Support model run that outputs a summary
</commit_message>
<xml_diff>
--- a/logic/test/data/_input/05_model_parameters/code_conversions.xlsx
+++ b/logic/test/data/_input/05_model_parameters/code_conversions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RMABuild\emap\logic\test\data\_input\05_model_parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E34B9D1-3F23-4EEC-997A-353F60565117}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49DEAD2A-97B3-4690-B8C2-5C879E2B87DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23160" yWindow="1630" windowWidth="13660" windowHeight="16840" xr2:uid="{12251410-17C7-4612-87CA-5DF1EC65E2D3}"/>
+    <workbookView xWindow="850" yWindow="-110" windowWidth="37660" windowHeight="21820" xr2:uid="{12251410-17C7-4612-87CA-5DF1EC65E2D3}"/>
   </bookViews>
   <sheets>
     <sheet name="pollutant" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="217">
   <si>
     <t>CO</t>
   </si>
@@ -685,6 +685,9 @@
   </si>
   <si>
     <t>PCDD/ PCDF</t>
+  </si>
+  <si>
+    <t>SO2</t>
   </si>
 </sst>
 </file>
@@ -755,8 +758,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8B39CD43-4866-4C3B-A178-A99FF32F0A59}" name="tbl_pollutant" displayName="tbl_pollutant" ref="A1:B40" totalsRowShown="0">
-  <autoFilter ref="A1:B40" xr:uid="{0DE66D0D-5368-447A-8271-C03336321777}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8B39CD43-4866-4C3B-A178-A99FF32F0A59}" name="tbl_pollutant" displayName="tbl_pollutant" ref="A1:B41" totalsRowShown="0">
+  <autoFilter ref="A1:B41" xr:uid="{0DE66D0D-5368-447A-8271-C03336321777}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{9514C98B-B8D5-45BC-ADB2-ACBD4CE319C1}" name="pollutant_code"/>
     <tableColumn id="2" xr3:uid="{2AE8A41A-C1EE-4738-B98A-B5A89D38B9B1}" name="pollutant_names"/>
@@ -1085,10 +1088,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{157BD3C6-51C2-4B17-80FA-10EB7A062B80}">
-  <dimension ref="A1:B40"/>
+  <dimension ref="A1:B41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1411,9 +1414,17 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
+        <v>11</v>
+      </c>
+      <c r="B40" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
         <v>35</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B41" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Support scanning CEIP spatial patterns
</commit_message>
<xml_diff>
--- a/logic/test/data/_input/05_model_parameters/code_conversions.xlsx
+++ b/logic/test/data/_input/05_model_parameters/code_conversions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RMABuild\emap\logic\test\data\_input\05_model_parameters\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Unit_RMA\MAP\_Modellen\E-MAP\05_Runs\_input\05_model_parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49DEAD2A-97B3-4690-B8C2-5C879E2B87DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4540633D-547D-424F-977F-B604DA12459E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="850" yWindow="-110" windowWidth="37660" windowHeight="21820" xr2:uid="{12251410-17C7-4612-87CA-5DF1EC65E2D3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{12251410-17C7-4612-87CA-5DF1EC65E2D3}"/>
   </bookViews>
   <sheets>
     <sheet name="pollutant" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="220">
   <si>
     <t>CO</t>
   </si>
@@ -675,19 +675,28 @@
     <t>NFR_priority</t>
   </si>
   <si>
+    <t>PCDD/ PCDF</t>
+  </si>
+  <si>
+    <t>benzo(b)</t>
+  </si>
+  <si>
+    <t>benzo(k)</t>
+  </si>
+  <si>
     <t>PCB</t>
   </si>
   <si>
-    <t>benzo(b)</t>
-  </si>
-  <si>
-    <t>benzo(k)</t>
-  </si>
-  <si>
-    <t>PCDD/ PCDF</t>
-  </si>
-  <si>
     <t>SO2</t>
+  </si>
+  <si>
+    <t>benzo(a)</t>
+  </si>
+  <si>
+    <t>PAH</t>
+  </si>
+  <si>
+    <t>DIOX</t>
   </si>
 </sst>
 </file>
@@ -758,11 +767,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8B39CD43-4866-4C3B-A178-A99FF32F0A59}" name="tbl_pollutant" displayName="tbl_pollutant" ref="A1:B41" totalsRowShown="0">
-  <autoFilter ref="A1:B41" xr:uid="{0DE66D0D-5368-447A-8271-C03336321777}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4A88631E-3733-463E-AE4E-37BF456FD3D8}" name="tbl_pollutant5" displayName="tbl_pollutant5" ref="A1:B44" totalsRowShown="0">
+  <autoFilter ref="A1:B44" xr:uid="{A508361B-4E71-4F87-8B57-2CE0238DA6A9}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{9514C98B-B8D5-45BC-ADB2-ACBD4CE319C1}" name="pollutant_code"/>
-    <tableColumn id="2" xr3:uid="{2AE8A41A-C1EE-4738-B98A-B5A89D38B9B1}" name="pollutant_names"/>
+    <tableColumn id="1" xr3:uid="{63BF32F6-EE9B-4E5C-8BB3-21FC917C2A74}" name="pollutant_code"/>
+    <tableColumn id="2" xr3:uid="{06197840-3C9F-4555-BD99-57AE89CFAE84}" name="pollutant_names"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -1088,19 +1097,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{157BD3C6-51C2-4B17-80FA-10EB7A062B80}">
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:B44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.7265625" customWidth="1"/>
-    <col min="2" max="2" width="27.26953125" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>40</v>
       </c>
@@ -1108,7 +1117,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1116,7 +1125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1124,7 +1133,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1132,7 +1141,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1140,7 +1149,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1148,7 +1157,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1156,7 +1165,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1164,7 +1173,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1172,7 +1181,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1180,7 +1189,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1188,7 +1197,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1196,7 +1205,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1204,7 +1213,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -1212,7 +1221,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -1220,7 +1229,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -1228,7 +1237,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -1236,7 +1245,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -1244,7 +1253,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -1252,7 +1261,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -1260,15 +1269,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -1276,7 +1285,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -1284,7 +1293,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -1292,7 +1301,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -1300,7 +1309,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>31</v>
       </c>
@@ -1308,7 +1317,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -1316,7 +1325,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>33</v>
       </c>
@@ -1324,7 +1333,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>35</v>
       </c>
@@ -1332,7 +1341,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>38</v>
       </c>
@@ -1340,7 +1349,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>39</v>
       </c>
@@ -1348,15 +1357,15 @@
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>39</v>
       </c>
       <c r="B32" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>2</v>
       </c>
@@ -1364,7 +1373,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>5</v>
       </c>
@@ -1372,7 +1381,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>2</v>
       </c>
@@ -1380,7 +1389,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>5</v>
       </c>
@@ -1388,7 +1397,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>9</v>
       </c>
@@ -1396,7 +1405,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>11</v>
       </c>
@@ -1404,7 +1413,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>11</v>
       </c>
@@ -1412,7 +1421,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>11</v>
       </c>
@@ -1420,12 +1429,36 @@
         <v>216</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>35</v>
       </c>
       <c r="B41" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>27</v>
+      </c>
+      <c r="B42" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>35</v>
+      </c>
+      <c r="B43" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>25</v>
+      </c>
+      <c r="B44" t="s">
+        <v>219</v>
       </c>
     </row>
   </sheetData>
@@ -1441,18 +1474,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F794111A-ABDF-4210-BBBE-1B707CBC36D1}">
   <dimension ref="A1:E135"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="F120" sqref="F120"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.1796875" customWidth="1"/>
-    <col min="2" max="2" width="13.54296875" customWidth="1"/>
-    <col min="3" max="3" width="14.1796875" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>169</v>
       </c>
@@ -1463,7 +1496,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>42</v>
       </c>
@@ -1477,7 +1510,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>43</v>
       </c>
@@ -1488,7 +1521,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>44</v>
       </c>
@@ -1499,7 +1532,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -1510,7 +1543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>46</v>
       </c>
@@ -1521,7 +1554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>47</v>
       </c>
@@ -1532,7 +1565,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>48</v>
       </c>
@@ -1543,7 +1576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>49</v>
       </c>
@@ -1554,7 +1587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>50</v>
       </c>
@@ -1565,7 +1598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>51</v>
       </c>
@@ -1576,7 +1609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>52</v>
       </c>
@@ -1587,7 +1620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>53</v>
       </c>
@@ -1598,7 +1631,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>54</v>
       </c>
@@ -1609,7 +1642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>55</v>
       </c>
@@ -1620,7 +1653,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>56</v>
       </c>
@@ -1631,7 +1664,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>57</v>
       </c>
@@ -1642,7 +1675,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>58</v>
       </c>
@@ -1653,7 +1686,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>59</v>
       </c>
@@ -1664,7 +1697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>60</v>
       </c>
@@ -1675,7 +1708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>61</v>
       </c>
@@ -1686,7 +1719,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>62</v>
       </c>
@@ -1697,7 +1730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>63</v>
       </c>
@@ -1708,7 +1741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>64</v>
       </c>
@@ -1719,7 +1752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>65</v>
       </c>
@@ -1730,7 +1763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>66</v>
       </c>
@@ -1741,7 +1774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>67</v>
       </c>
@@ -1752,7 +1785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>68</v>
       </c>
@@ -1763,7 +1796,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>69</v>
       </c>
@@ -1774,7 +1807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>70</v>
       </c>
@@ -1785,7 +1818,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>71</v>
       </c>
@@ -1796,7 +1829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>72</v>
       </c>
@@ -1807,7 +1840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>73</v>
       </c>
@@ -1818,7 +1851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>74</v>
       </c>
@@ -1829,7 +1862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>75</v>
       </c>
@@ -1840,7 +1873,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>76</v>
       </c>
@@ -1851,7 +1884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>77</v>
       </c>
@@ -1862,7 +1895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>78</v>
       </c>
@@ -1873,7 +1906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>79</v>
       </c>
@@ -1884,7 +1917,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>80</v>
       </c>
@@ -1895,7 +1928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>81</v>
       </c>
@@ -1906,7 +1939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>82</v>
       </c>
@@ -1917,7 +1950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>83</v>
       </c>
@@ -1928,7 +1961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>84</v>
       </c>
@@ -1939,7 +1972,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>85</v>
       </c>
@@ -1950,7 +1983,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>86</v>
       </c>
@@ -1961,7 +1994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>87</v>
       </c>
@@ -1972,7 +2005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>88</v>
       </c>
@@ -1983,7 +2016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>89</v>
       </c>
@@ -1994,7 +2027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>90</v>
       </c>
@@ -2005,7 +2038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>91</v>
       </c>
@@ -2016,7 +2049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>92</v>
       </c>
@@ -2027,7 +2060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>93</v>
       </c>
@@ -2038,7 +2071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>94</v>
       </c>
@@ -2049,7 +2082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>95</v>
       </c>
@@ -2060,7 +2093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>96</v>
       </c>
@@ -2071,7 +2104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>97</v>
       </c>
@@ -2082,7 +2115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>98</v>
       </c>
@@ -2093,7 +2126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>99</v>
       </c>
@@ -2104,7 +2137,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>100</v>
       </c>
@@ -2115,7 +2148,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>101</v>
       </c>
@@ -2126,7 +2159,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>102</v>
       </c>
@@ -2137,7 +2170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>103</v>
       </c>
@@ -2148,7 +2181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>104</v>
       </c>
@@ -2159,7 +2192,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>105</v>
       </c>
@@ -2170,7 +2203,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>106</v>
       </c>
@@ -2181,7 +2214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>107</v>
       </c>
@@ -2192,7 +2225,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>108</v>
       </c>
@@ -2203,7 +2236,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>109</v>
       </c>
@@ -2214,7 +2247,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>110</v>
       </c>
@@ -2225,7 +2258,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>111</v>
       </c>
@@ -2236,7 +2269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>112</v>
       </c>
@@ -2247,7 +2280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>113</v>
       </c>
@@ -2258,7 +2291,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>114</v>
       </c>
@@ -2269,7 +2302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>115</v>
       </c>
@@ -2280,7 +2313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>116</v>
       </c>
@@ -2291,7 +2324,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>117</v>
       </c>
@@ -2302,7 +2335,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>118</v>
       </c>
@@ -2313,7 +2346,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>119</v>
       </c>
@@ -2324,7 +2357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>120</v>
       </c>
@@ -2335,7 +2368,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>121</v>
       </c>
@@ -2346,7 +2379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>122</v>
       </c>
@@ -2357,7 +2390,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>123</v>
       </c>
@@ -2368,7 +2401,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>124</v>
       </c>
@@ -2379,7 +2412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>125</v>
       </c>
@@ -2390,7 +2423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>126</v>
       </c>
@@ -2401,7 +2434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>127</v>
       </c>
@@ -2412,7 +2445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>128</v>
       </c>
@@ -2423,7 +2456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>129</v>
       </c>
@@ -2434,7 +2467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>130</v>
       </c>
@@ -2445,7 +2478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>131</v>
       </c>
@@ -2456,7 +2489,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>132</v>
       </c>
@@ -2467,7 +2500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>133</v>
       </c>
@@ -2478,7 +2511,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>134</v>
       </c>
@@ -2489,7 +2522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>135</v>
       </c>
@@ -2500,7 +2533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>136</v>
       </c>
@@ -2511,7 +2544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>137</v>
       </c>
@@ -2522,7 +2555,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>138</v>
       </c>
@@ -2533,7 +2566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>139</v>
       </c>
@@ -2544,7 +2577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>140</v>
       </c>
@@ -2555,7 +2588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>141</v>
       </c>
@@ -2566,7 +2599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>142</v>
       </c>
@@ -2577,7 +2610,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>143</v>
       </c>
@@ -2588,7 +2621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>144</v>
       </c>
@@ -2599,7 +2632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>145</v>
       </c>
@@ -2610,7 +2643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>146</v>
       </c>
@@ -2621,7 +2654,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>147</v>
       </c>
@@ -2632,7 +2665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>148</v>
       </c>
@@ -2643,7 +2676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>149</v>
       </c>
@@ -2654,7 +2687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>150</v>
       </c>
@@ -2665,7 +2698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>151</v>
       </c>
@@ -2676,7 +2709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>152</v>
       </c>
@@ -2687,7 +2720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>153</v>
       </c>
@@ -2698,7 +2731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>154</v>
       </c>
@@ -2709,7 +2742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>155</v>
       </c>
@@ -2720,7 +2753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>156</v>
       </c>
@@ -2731,7 +2764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>157</v>
       </c>
@@ -2742,7 +2775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>158</v>
       </c>
@@ -2753,7 +2786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>159</v>
       </c>
@@ -2764,7 +2797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>160</v>
       </c>
@@ -2775,7 +2808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>161</v>
       </c>
@@ -2786,7 +2819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>162</v>
       </c>
@@ -2797,7 +2830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>163</v>
       </c>
@@ -2808,7 +2841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>164</v>
       </c>
@@ -2819,7 +2852,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>165</v>
       </c>
@@ -2830,7 +2863,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>166</v>
       </c>
@@ -2841,7 +2874,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>167</v>
       </c>
@@ -2852,7 +2885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>168</v>
       </c>
@@ -2863,7 +2896,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>55</v>
       </c>
@@ -2874,7 +2907,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>56</v>
       </c>
@@ -2885,7 +2918,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>57</v>
       </c>
@@ -2896,7 +2929,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>58</v>
       </c>
@@ -2907,7 +2940,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>59</v>
       </c>
@@ -2918,7 +2951,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>60</v>
       </c>
@@ -2929,7 +2962,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>61</v>
       </c>
@@ -2956,13 +2989,13 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.453125" customWidth="1"/>
-    <col min="2" max="2" width="27.81640625" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>184</v>
       </c>
@@ -2970,7 +3003,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>186</v>
       </c>
@@ -2978,7 +3011,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>187</v>
       </c>
@@ -2986,7 +3019,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>188</v>
       </c>
@@ -2994,7 +3027,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>188</v>
       </c>
@@ -3002,7 +3035,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>189</v>
       </c>
@@ -3010,7 +3043,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>189</v>
       </c>
@@ -3018,7 +3051,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>190</v>
       </c>
@@ -3026,7 +3059,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>191</v>
       </c>
@@ -3034,7 +3067,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>192</v>
       </c>
@@ -3042,7 +3075,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>193</v>
       </c>
@@ -3050,7 +3083,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>194</v>
       </c>
@@ -3058,7 +3091,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>195</v>
       </c>
@@ -3066,7 +3099,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>196</v>
       </c>
@@ -3074,7 +3107,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>197</v>
       </c>
@@ -3082,7 +3115,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>198</v>
       </c>
@@ -3090,7 +3123,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>196</v>
       </c>

</xml_diff>

<commit_message>
Fixed sector numbers in output
</commit_message>
<xml_diff>
--- a/logic/test/data/_input/05_model_parameters/code_conversions.xlsx
+++ b/logic/test/data/_input/05_model_parameters/code_conversions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Unit_RMA\MAP\_Modellen\E-MAP\05_Runs\_input\05_model_parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4540633D-547D-424F-977F-B604DA12459E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{41892AC5-A32E-40AE-BC96-B8211A3BA78A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{12251410-17C7-4612-87CA-5DF1EC65E2D3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{12251410-17C7-4612-87CA-5DF1EC65E2D3}"/>
   </bookViews>
   <sheets>
     <sheet name="pollutant" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="222">
   <si>
     <t>CO</t>
   </si>
@@ -697,6 +697,12 @@
   </si>
   <si>
     <t>DIOX</t>
+  </si>
+  <si>
+    <t>covnm</t>
+  </si>
+  <si>
+    <t>1A3bviii</t>
   </si>
 </sst>
 </file>
@@ -767,8 +773,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4A88631E-3733-463E-AE4E-37BF456FD3D8}" name="tbl_pollutant5" displayName="tbl_pollutant5" ref="A1:B44" totalsRowShown="0">
-  <autoFilter ref="A1:B44" xr:uid="{A508361B-4E71-4F87-8B57-2CE0238DA6A9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4A88631E-3733-463E-AE4E-37BF456FD3D8}" name="tbl_pollutant5" displayName="tbl_pollutant5" ref="A1:B45" totalsRowShown="0">
+  <autoFilter ref="A1:B45" xr:uid="{A508361B-4E71-4F87-8B57-2CE0238DA6A9}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{63BF32F6-EE9B-4E5C-8BB3-21FC917C2A74}" name="pollutant_code"/>
     <tableColumn id="2" xr3:uid="{06197840-3C9F-4555-BD99-57AE89CFAE84}" name="pollutant_names"/>
@@ -778,8 +784,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FDCE720D-A617-4F5B-8433-85E2C6857173}" name="tbl_NFR" displayName="tbl_NFR" ref="A1:C135" totalsRowShown="0">
-  <autoFilter ref="A1:C135" xr:uid="{BD0EA715-BDB1-4D0E-80B6-1F3E5150B3C3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FDCE720D-A617-4F5B-8433-85E2C6857173}" name="tbl_NFR" displayName="tbl_NFR" ref="A1:C136" totalsRowShown="0">
+  <autoFilter ref="A1:C136" xr:uid="{BD0EA715-BDB1-4D0E-80B6-1F3E5150B3C3}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{6B25390A-63E3-40F9-84C1-A7A2AC040592}" name="NFR_code"/>
     <tableColumn id="2" xr3:uid="{ECCCA51A-7F4A-4651-8972-626FD9996640}" name="NFR_names"/>
@@ -1097,10 +1103,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{157BD3C6-51C2-4B17-80FA-10EB7A062B80}">
-  <dimension ref="A1:B44"/>
+  <dimension ref="A1:B45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1461,6 +1467,14 @@
         <v>219</v>
       </c>
     </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>2</v>
+      </c>
+      <c r="B45" t="s">
+        <v>220</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="128" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1472,11 +1486,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F794111A-ABDF-4210-BBBE-1B707CBC36D1}">
-  <dimension ref="A1:E135"/>
+  <dimension ref="A1:E136"/>
   <sheetViews>
-    <sheetView topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="F120" sqref="F120"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2971,6 +2983,17 @@
       </c>
       <c r="C135">
         <v>2</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>221</v>
+      </c>
+      <c r="B136" t="s">
+        <v>221</v>
+      </c>
+      <c r="C136">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Use a faster csv parser to parse the point sources
</commit_message>
<xml_diff>
--- a/logic/test/data/_input/05_model_parameters/code_conversions.xlsx
+++ b/logic/test/data/_input/05_model_parameters/code_conversions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Unit_RMA\MAP\_Modellen\E-MAP\05_Runs\_input\05_model_parameters\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RMABuild\emap\logic\test\data\_input\05_model_parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{41892AC5-A32E-40AE-BC96-B8211A3BA78A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14211100-A259-4E05-9212-189830B8F96C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{12251410-17C7-4612-87CA-5DF1EC65E2D3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{12251410-17C7-4612-87CA-5DF1EC65E2D3}"/>
   </bookViews>
   <sheets>
     <sheet name="pollutant" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="223">
   <si>
     <t>CO</t>
   </si>
@@ -703,6 +703,9 @@
   </si>
   <si>
     <t>1A3bviii</t>
+  </si>
+  <si>
+    <t>NO2</t>
   </si>
 </sst>
 </file>
@@ -773,8 +776,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4A88631E-3733-463E-AE4E-37BF456FD3D8}" name="tbl_pollutant5" displayName="tbl_pollutant5" ref="A1:B45" totalsRowShown="0">
-  <autoFilter ref="A1:B45" xr:uid="{A508361B-4E71-4F87-8B57-2CE0238DA6A9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4A88631E-3733-463E-AE4E-37BF456FD3D8}" name="tbl_pollutant5" displayName="tbl_pollutant5" ref="A1:B46" totalsRowShown="0">
+  <autoFilter ref="A1:B46" xr:uid="{A508361B-4E71-4F87-8B57-2CE0238DA6A9}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{63BF32F6-EE9B-4E5C-8BB3-21FC917C2A74}" name="pollutant_code"/>
     <tableColumn id="2" xr3:uid="{06197840-3C9F-4555-BD99-57AE89CFAE84}" name="pollutant_names"/>
@@ -1103,19 +1106,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{157BD3C6-51C2-4B17-80FA-10EB7A062B80}">
-  <dimension ref="A1:B45"/>
+  <dimension ref="A1:B46"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" customWidth="1"/>
-    <col min="2" max="2" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5546875" customWidth="1"/>
+    <col min="2" max="2" width="26.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>40</v>
       </c>
@@ -1123,7 +1126,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1131,7 +1134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1139,7 +1142,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1147,7 +1150,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1155,7 +1158,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1163,7 +1166,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1171,7 +1174,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1179,7 +1182,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1187,7 +1190,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1195,7 +1198,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1203,7 +1206,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1211,7 +1214,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1219,7 +1222,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -1227,7 +1230,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -1235,7 +1238,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -1243,7 +1246,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -1251,7 +1254,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -1259,7 +1262,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -1267,7 +1270,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -1275,7 +1278,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -1283,7 +1286,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -1291,7 +1294,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -1299,7 +1302,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -1307,7 +1310,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -1315,7 +1318,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>31</v>
       </c>
@@ -1323,7 +1326,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -1331,7 +1334,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>33</v>
       </c>
@@ -1339,7 +1342,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>35</v>
       </c>
@@ -1347,7 +1350,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>38</v>
       </c>
@@ -1355,7 +1358,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>39</v>
       </c>
@@ -1363,7 +1366,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>39</v>
       </c>
@@ -1371,7 +1374,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>2</v>
       </c>
@@ -1379,7 +1382,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>5</v>
       </c>
@@ -1387,7 +1390,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>2</v>
       </c>
@@ -1395,7 +1398,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>5</v>
       </c>
@@ -1403,75 +1406,83 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
+        <v>5</v>
+      </c>
+      <c r="B37" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
         <v>9</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>11</v>
-      </c>
-      <c r="B38" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>11</v>
       </c>
       <c r="B39" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>11</v>
       </c>
       <c r="B40" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>11</v>
+      </c>
+      <c r="B41" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
         <v>35</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B42" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
         <v>27</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B43" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
         <v>35</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B44" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
         <v>25</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
         <v>2</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B46" t="s">
         <v>220</v>
       </c>
     </row>
@@ -1488,16 +1499,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F794111A-ABDF-4210-BBBE-1B707CBC36D1}">
   <dimension ref="A1:E136"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" customWidth="1"/>
+    <col min="1" max="1" width="19.109375" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>169</v>
       </c>
@@ -1508,7 +1519,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>42</v>
       </c>
@@ -1522,7 +1533,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>43</v>
       </c>
@@ -1533,7 +1544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>44</v>
       </c>
@@ -1544,7 +1555,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -1555,7 +1566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>46</v>
       </c>
@@ -1566,7 +1577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>47</v>
       </c>
@@ -1577,7 +1588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>48</v>
       </c>
@@ -1588,7 +1599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>49</v>
       </c>
@@ -1599,7 +1610,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>50</v>
       </c>
@@ -1610,7 +1621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>51</v>
       </c>
@@ -1621,7 +1632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>52</v>
       </c>
@@ -1632,7 +1643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>53</v>
       </c>
@@ -1643,7 +1654,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>54</v>
       </c>
@@ -1654,7 +1665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>55</v>
       </c>
@@ -1665,7 +1676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>56</v>
       </c>
@@ -1676,7 +1687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>57</v>
       </c>
@@ -1687,7 +1698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>58</v>
       </c>
@@ -1698,7 +1709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>59</v>
       </c>
@@ -1709,7 +1720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>60</v>
       </c>
@@ -1720,7 +1731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>61</v>
       </c>
@@ -1731,7 +1742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>62</v>
       </c>
@@ -1742,7 +1753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>63</v>
       </c>
@@ -1753,7 +1764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>64</v>
       </c>
@@ -1764,7 +1775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>65</v>
       </c>
@@ -1775,7 +1786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>66</v>
       </c>
@@ -1786,7 +1797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>67</v>
       </c>
@@ -1797,7 +1808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>68</v>
       </c>
@@ -1808,7 +1819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>69</v>
       </c>
@@ -1819,7 +1830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>70</v>
       </c>
@@ -1830,7 +1841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>71</v>
       </c>
@@ -1841,7 +1852,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>72</v>
       </c>
@@ -1852,7 +1863,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>73</v>
       </c>
@@ -1863,7 +1874,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>74</v>
       </c>
@@ -1874,7 +1885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>75</v>
       </c>
@@ -1885,7 +1896,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>76</v>
       </c>
@@ -1896,7 +1907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>77</v>
       </c>
@@ -1907,7 +1918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>78</v>
       </c>
@@ -1918,7 +1929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>79</v>
       </c>
@@ -1929,7 +1940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>80</v>
       </c>
@@ -1940,7 +1951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>81</v>
       </c>
@@ -1951,7 +1962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>82</v>
       </c>
@@ -1962,7 +1973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>83</v>
       </c>
@@ -1973,7 +1984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>84</v>
       </c>
@@ -1984,7 +1995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>85</v>
       </c>
@@ -1995,7 +2006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>86</v>
       </c>
@@ -2006,7 +2017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>87</v>
       </c>
@@ -2017,7 +2028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>88</v>
       </c>
@@ -2028,7 +2039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>89</v>
       </c>
@@ -2039,7 +2050,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>90</v>
       </c>
@@ -2050,7 +2061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>91</v>
       </c>
@@ -2061,7 +2072,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>92</v>
       </c>
@@ -2072,7 +2083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>93</v>
       </c>
@@ -2083,7 +2094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>94</v>
       </c>
@@ -2094,7 +2105,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>95</v>
       </c>
@@ -2105,7 +2116,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>96</v>
       </c>
@@ -2116,7 +2127,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>97</v>
       </c>
@@ -2127,7 +2138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>98</v>
       </c>
@@ -2138,7 +2149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>99</v>
       </c>
@@ -2149,7 +2160,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>100</v>
       </c>
@@ -2160,7 +2171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>101</v>
       </c>
@@ -2171,7 +2182,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>102</v>
       </c>
@@ -2182,7 +2193,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>103</v>
       </c>
@@ -2193,7 +2204,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>104</v>
       </c>
@@ -2204,7 +2215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>105</v>
       </c>
@@ -2215,7 +2226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>106</v>
       </c>
@@ -2226,7 +2237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>107</v>
       </c>
@@ -2237,7 +2248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>108</v>
       </c>
@@ -2248,7 +2259,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>109</v>
       </c>
@@ -2259,7 +2270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>110</v>
       </c>
@@ -2270,7 +2281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>111</v>
       </c>
@@ -2281,7 +2292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>112</v>
       </c>
@@ -2292,7 +2303,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>113</v>
       </c>
@@ -2303,7 +2314,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>114</v>
       </c>
@@ -2314,7 +2325,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>115</v>
       </c>
@@ -2325,7 +2336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>116</v>
       </c>
@@ -2336,7 +2347,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>117</v>
       </c>
@@ -2347,7 +2358,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>118</v>
       </c>
@@ -2358,7 +2369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>119</v>
       </c>
@@ -2369,7 +2380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>120</v>
       </c>
@@ -2380,7 +2391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>121</v>
       </c>
@@ -2391,7 +2402,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>122</v>
       </c>
@@ -2402,7 +2413,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>123</v>
       </c>
@@ -2413,7 +2424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>124</v>
       </c>
@@ -2424,7 +2435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>125</v>
       </c>
@@ -2435,7 +2446,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>126</v>
       </c>
@@ -2446,7 +2457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>127</v>
       </c>
@@ -2457,7 +2468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>128</v>
       </c>
@@ -2468,7 +2479,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>129</v>
       </c>
@@ -2479,7 +2490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>130</v>
       </c>
@@ -2490,7 +2501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>131</v>
       </c>
@@ -2501,7 +2512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>132</v>
       </c>
@@ -2512,7 +2523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>133</v>
       </c>
@@ -2523,7 +2534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>134</v>
       </c>
@@ -2534,7 +2545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>135</v>
       </c>
@@ -2545,7 +2556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>136</v>
       </c>
@@ -2556,7 +2567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>137</v>
       </c>
@@ -2567,7 +2578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>138</v>
       </c>
@@ -2578,7 +2589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>139</v>
       </c>
@@ -2589,7 +2600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>140</v>
       </c>
@@ -2600,7 +2611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>141</v>
       </c>
@@ -2611,7 +2622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>142</v>
       </c>
@@ -2622,7 +2633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>143</v>
       </c>
@@ -2633,7 +2644,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>144</v>
       </c>
@@ -2644,7 +2655,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>145</v>
       </c>
@@ -2655,7 +2666,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>146</v>
       </c>
@@ -2666,7 +2677,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>147</v>
       </c>
@@ -2677,7 +2688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>148</v>
       </c>
@@ -2688,7 +2699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>149</v>
       </c>
@@ -2699,7 +2710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>150</v>
       </c>
@@ -2710,7 +2721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>151</v>
       </c>
@@ -2721,7 +2732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>152</v>
       </c>
@@ -2732,7 +2743,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>153</v>
       </c>
@@ -2743,7 +2754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>154</v>
       </c>
@@ -2754,7 +2765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>155</v>
       </c>
@@ -2765,7 +2776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>156</v>
       </c>
@@ -2776,7 +2787,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>157</v>
       </c>
@@ -2787,7 +2798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>158</v>
       </c>
@@ -2798,7 +2809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>159</v>
       </c>
@@ -2809,7 +2820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>160</v>
       </c>
@@ -2820,7 +2831,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>161</v>
       </c>
@@ -2831,7 +2842,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>162</v>
       </c>
@@ -2842,7 +2853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>163</v>
       </c>
@@ -2853,7 +2864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>164</v>
       </c>
@@ -2864,7 +2875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>165</v>
       </c>
@@ -2875,7 +2886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>166</v>
       </c>
@@ -2886,7 +2897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>167</v>
       </c>
@@ -2897,7 +2908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>168</v>
       </c>
@@ -2908,7 +2919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>55</v>
       </c>
@@ -2919,7 +2930,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>56</v>
       </c>
@@ -2930,7 +2941,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>57</v>
       </c>
@@ -2941,7 +2952,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>58</v>
       </c>
@@ -2952,7 +2963,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>59</v>
       </c>
@@ -2963,7 +2974,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>60</v>
       </c>
@@ -2974,7 +2985,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>61</v>
       </c>
@@ -2985,7 +2996,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>221</v>
       </c>
@@ -3012,13 +3023,13 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="1"/>
-    <col min="2" max="2" width="27.85546875" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" customWidth="1"/>
+    <col min="2" max="2" width="27.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>184</v>
       </c>
@@ -3026,7 +3037,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>186</v>
       </c>
@@ -3034,7 +3045,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>187</v>
       </c>
@@ -3042,7 +3053,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>188</v>
       </c>
@@ -3050,7 +3061,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>188</v>
       </c>
@@ -3058,7 +3069,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>189</v>
       </c>
@@ -3066,7 +3077,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>189</v>
       </c>
@@ -3074,7 +3085,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>190</v>
       </c>
@@ -3082,7 +3093,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>191</v>
       </c>
@@ -3090,7 +3101,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>192</v>
       </c>
@@ -3098,7 +3109,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>193</v>
       </c>
@@ -3106,7 +3117,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>194</v>
       </c>
@@ -3114,7 +3125,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>195</v>
       </c>
@@ -3122,7 +3133,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>196</v>
       </c>
@@ -3130,7 +3141,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>197</v>
       </c>
@@ -3138,7 +3149,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>198</v>
       </c>
@@ -3146,7 +3157,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>196</v>
       </c>

</xml_diff>